<commit_message>
Se agregaron las clausulas necesarias para la uditoria, ademas se adjutaron las clausulas que no funcionan en el proyecto
</commit_message>
<xml_diff>
--- a/09_Programa_aud_interno/PROGRAMA_AUDI_INTERNA_G8_V2.xlsx
+++ b/09_Programa_aud_interno/PROGRAMA_AUDI_INTERNA_G8_V2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\UsuarioLVD\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shadow Moon\Desktop\Universidad\Septimo Semestre\Aseguramiento de la Calidad\git\2563_G8_ACSW\09_Programa_aud_interno\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9424A318-8096-4D1A-A5DF-785BD9100FAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F82A43C-ABF8-488E-8C4C-907547A45746}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1. PROGRAMA" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="116">
   <si>
     <t>Fecha de Emisión:</t>
   </si>
@@ -533,6 +533,78 @@
 Exportación del Reporte:
 Genera un informe en formato PDF o HTML para compartir con los stakeholders.
 Incluir: resumen del estado, defectos encontrados, áreas críticas identificadas.</t>
+  </si>
+  <si>
+    <t>11:00
+13:01</t>
+  </si>
+  <si>
+    <t>ISO-ICE-IEEE-29119-6</t>
+  </si>
+  <si>
+    <t>Permite mitigar problemas antes de que impacten el desarrollo, una práctica esencial en entornos con requisitos estrictos o alta incertidumbre.</t>
+  </si>
+  <si>
+    <t>6.2.6</t>
+  </si>
+  <si>
+    <t>11:00
+13:02</t>
+  </si>
+  <si>
+    <t>ISO-ICE-IEEE-29119-7</t>
+  </si>
+  <si>
+    <t>El proyecto incluye pruebas automatizadas o integraciones complejas, definir esto ayuda a alinear expectativas y minimizar problemas técnicos.</t>
+  </si>
+  <si>
+    <t>6.2.7</t>
+  </si>
+  <si>
+    <t>11:00
+13:03</t>
+  </si>
+  <si>
+    <t>ISO-ICE-IEEE-29119-8</t>
+  </si>
+  <si>
+    <t>El proyecto tiene restricciones de tiempo, esto es crucial para coordinar las entregas y el progreso.</t>
+  </si>
+  <si>
+    <t>6.2.10</t>
+  </si>
+  <si>
+    <t>El equipo está definido desde el inicio y no hay necesidad de contratar personal adicional, esta cláusula es irrelevante.</t>
+  </si>
+  <si>
+    <t>6.2.9</t>
+  </si>
+  <si>
+    <t>Las pruebas no son críticas para el lanzamiento (por ejemplo, no se trata de un sistema de misión crítica), estos criterios pueden no ser necesarios.</t>
+  </si>
+  <si>
+    <t>6.2.7.9</t>
+  </si>
+  <si>
+    <t>En proyectos donde las funcionalidades son simples y no hay dependencias significativas entre módulos, estas actividades podrían no ser necesarias.</t>
+  </si>
+  <si>
+    <t>6.2.7.8</t>
+  </si>
+  <si>
+    <t>Si los datos de prueba son básicos o están integrados directamente en el software sin mayores complejidades, esta sección podría omitirse.</t>
+  </si>
+  <si>
+    <t>6.2.7.6</t>
+  </si>
+  <si>
+    <t>El proyecto se encuentra en un entorno pequeño y las pruebas realizadas son en una sola máquina.</t>
+  </si>
+  <si>
+    <t>6.2.7.7</t>
+  </si>
+  <si>
+    <t>CLAUSULAS QUE NO SE UTILIZARAN EN LAS PRUEBAS DEL PROYECTO</t>
   </si>
 </sst>
 </file>
@@ -1301,7 +1373,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="160">
+  <cellXfs count="159">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1513,14 +1585,19 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1530,14 +1607,24 @@
     <xf numFmtId="0" fontId="22" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -1548,7 +1635,61 @@
     <xf numFmtId="0" fontId="17" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="10" fontId="20" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="16" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="16" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="16" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1562,9 +1703,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1588,75 +1726,22 @@
     <xf numFmtId="49" fontId="14" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="20" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="16" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="16" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="16" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -1671,20 +1756,8 @@
     <xf numFmtId="0" fontId="35" fillId="6" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="35" fillId="6" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1943,27 +2016,27 @@
   </sheetPr>
   <dimension ref="A1:AQ1000"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="B24" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
       <selection activeCell="AJ7" sqref="AJ7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="12.7109375" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="3.28515625" customWidth="1"/>
-    <col min="2" max="2" width="5.28515625" customWidth="1"/>
+    <col min="1" max="1" width="3.33203125" customWidth="1"/>
+    <col min="2" max="2" width="5.33203125" customWidth="1"/>
     <col min="3" max="3" width="29" customWidth="1"/>
-    <col min="4" max="4" width="4.85546875" customWidth="1"/>
-    <col min="5" max="5" width="8.28515625" customWidth="1"/>
-    <col min="6" max="6" width="7.28515625" customWidth="1"/>
+    <col min="4" max="4" width="4.88671875" customWidth="1"/>
+    <col min="5" max="5" width="8.33203125" customWidth="1"/>
+    <col min="6" max="6" width="7.33203125" customWidth="1"/>
     <col min="7" max="7" width="7" customWidth="1"/>
-    <col min="8" max="8" width="19.140625" customWidth="1"/>
+    <col min="8" max="8" width="19.109375" customWidth="1"/>
     <col min="9" max="20" width="7" customWidth="1"/>
-    <col min="21" max="21" width="9.7109375" customWidth="1"/>
-    <col min="22" max="22" width="60.28515625" customWidth="1"/>
-    <col min="23" max="23" width="28.7109375" customWidth="1"/>
-    <col min="24" max="36" width="1.28515625" customWidth="1"/>
-    <col min="37" max="37" width="17.28515625" customWidth="1"/>
-    <col min="38" max="43" width="11.28515625" customWidth="1"/>
+    <col min="21" max="21" width="9.6640625" customWidth="1"/>
+    <col min="22" max="22" width="60.33203125" customWidth="1"/>
+    <col min="23" max="23" width="28.6640625" customWidth="1"/>
+    <col min="24" max="36" width="1.33203125" customWidth="1"/>
+    <col min="37" max="37" width="17.33203125" customWidth="1"/>
+    <col min="38" max="43" width="11.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:43" ht="12.75" customHeight="1">
@@ -1971,32 +2044,32 @@
     </row>
     <row r="2" spans="1:43" ht="42.75" customHeight="1">
       <c r="A2" s="2"/>
-      <c r="B2" s="128"/>
-      <c r="C2" s="129"/>
-      <c r="D2" s="129"/>
-      <c r="E2" s="129"/>
-      <c r="F2" s="130"/>
-      <c r="G2" s="131"/>
-      <c r="H2" s="120"/>
-      <c r="I2" s="120"/>
-      <c r="J2" s="120"/>
-      <c r="K2" s="120"/>
-      <c r="L2" s="120"/>
-      <c r="M2" s="121"/>
-      <c r="N2" s="126" t="s">
+      <c r="B2" s="109"/>
+      <c r="C2" s="87"/>
+      <c r="D2" s="87"/>
+      <c r="E2" s="87"/>
+      <c r="F2" s="94"/>
+      <c r="G2" s="111"/>
+      <c r="H2" s="84"/>
+      <c r="I2" s="84"/>
+      <c r="J2" s="84"/>
+      <c r="K2" s="84"/>
+      <c r="L2" s="84"/>
+      <c r="M2" s="85"/>
+      <c r="N2" s="112" t="s">
         <v>0</v>
       </c>
-      <c r="O2" s="120"/>
-      <c r="P2" s="120"/>
-      <c r="Q2" s="120"/>
-      <c r="R2" s="120"/>
-      <c r="S2" s="120"/>
-      <c r="T2" s="121"/>
-      <c r="U2" s="132">
+      <c r="O2" s="84"/>
+      <c r="P2" s="84"/>
+      <c r="Q2" s="84"/>
+      <c r="R2" s="84"/>
+      <c r="S2" s="84"/>
+      <c r="T2" s="85"/>
+      <c r="U2" s="113">
         <v>45644</v>
       </c>
-      <c r="V2" s="158"/>
-      <c r="W2" s="159"/>
+      <c r="V2" s="114"/>
+      <c r="W2" s="115"/>
       <c r="X2" s="2"/>
       <c r="Y2" s="2"/>
       <c r="Z2" s="2"/>
@@ -2020,32 +2093,32 @@
     </row>
     <row r="3" spans="1:43" ht="48.75" customHeight="1">
       <c r="A3" s="2"/>
-      <c r="B3" s="104"/>
-      <c r="C3" s="105"/>
-      <c r="D3" s="105"/>
-      <c r="E3" s="105"/>
+      <c r="B3" s="110"/>
+      <c r="C3" s="89"/>
+      <c r="D3" s="89"/>
+      <c r="E3" s="89"/>
       <c r="F3" s="106"/>
-      <c r="G3" s="133"/>
-      <c r="H3" s="120"/>
-      <c r="I3" s="120"/>
-      <c r="J3" s="120"/>
-      <c r="K3" s="120"/>
-      <c r="L3" s="120"/>
-      <c r="M3" s="121"/>
-      <c r="N3" s="125" t="s">
+      <c r="G3" s="116"/>
+      <c r="H3" s="84"/>
+      <c r="I3" s="84"/>
+      <c r="J3" s="84"/>
+      <c r="K3" s="84"/>
+      <c r="L3" s="84"/>
+      <c r="M3" s="85"/>
+      <c r="N3" s="117" t="s">
         <v>1</v>
       </c>
-      <c r="O3" s="120"/>
-      <c r="P3" s="120"/>
-      <c r="Q3" s="120"/>
-      <c r="R3" s="120"/>
-      <c r="S3" s="120"/>
-      <c r="T3" s="121"/>
-      <c r="U3" s="132">
+      <c r="O3" s="84"/>
+      <c r="P3" s="84"/>
+      <c r="Q3" s="84"/>
+      <c r="R3" s="84"/>
+      <c r="S3" s="84"/>
+      <c r="T3" s="85"/>
+      <c r="U3" s="113">
         <v>45665</v>
       </c>
-      <c r="V3" s="120"/>
-      <c r="W3" s="121"/>
+      <c r="V3" s="84"/>
+      <c r="W3" s="85"/>
       <c r="X3" s="2"/>
       <c r="Y3" s="2"/>
       <c r="Z3" s="2"/>
@@ -2069,34 +2142,34 @@
     </row>
     <row r="4" spans="1:43" ht="21" customHeight="1">
       <c r="A4" s="2"/>
-      <c r="B4" s="123" t="s">
+      <c r="B4" s="118" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="120"/>
-      <c r="D4" s="120"/>
-      <c r="E4" s="120"/>
-      <c r="F4" s="121"/>
-      <c r="G4" s="124"/>
-      <c r="H4" s="120"/>
-      <c r="I4" s="120"/>
-      <c r="J4" s="120"/>
-      <c r="K4" s="120"/>
-      <c r="L4" s="120"/>
-      <c r="M4" s="121"/>
-      <c r="N4" s="125" t="s">
+      <c r="C4" s="84"/>
+      <c r="D4" s="84"/>
+      <c r="E4" s="84"/>
+      <c r="F4" s="85"/>
+      <c r="G4" s="119"/>
+      <c r="H4" s="84"/>
+      <c r="I4" s="84"/>
+      <c r="J4" s="84"/>
+      <c r="K4" s="84"/>
+      <c r="L4" s="84"/>
+      <c r="M4" s="85"/>
+      <c r="N4" s="117" t="s">
         <v>3</v>
       </c>
-      <c r="O4" s="120"/>
-      <c r="P4" s="120"/>
-      <c r="Q4" s="120"/>
-      <c r="R4" s="120"/>
-      <c r="S4" s="120"/>
-      <c r="T4" s="121"/>
-      <c r="U4" s="126" t="s">
+      <c r="O4" s="84"/>
+      <c r="P4" s="84"/>
+      <c r="Q4" s="84"/>
+      <c r="R4" s="84"/>
+      <c r="S4" s="84"/>
+      <c r="T4" s="85"/>
+      <c r="U4" s="112" t="s">
         <v>4</v>
       </c>
-      <c r="V4" s="120"/>
-      <c r="W4" s="121"/>
+      <c r="V4" s="84"/>
+      <c r="W4" s="85"/>
       <c r="X4" s="2"/>
       <c r="Y4" s="2"/>
       <c r="Z4" s="2"/>
@@ -2164,30 +2237,30 @@
       <c r="AQ5" s="2"/>
     </row>
     <row r="6" spans="1:43" ht="20.25" customHeight="1">
-      <c r="B6" s="127" t="s">
+      <c r="B6" s="120" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="86"/>
-      <c r="D6" s="86"/>
-      <c r="E6" s="86"/>
-      <c r="F6" s="86"/>
-      <c r="G6" s="86"/>
-      <c r="H6" s="86"/>
-      <c r="I6" s="86"/>
-      <c r="J6" s="86"/>
-      <c r="K6" s="86"/>
-      <c r="L6" s="86"/>
-      <c r="M6" s="86"/>
-      <c r="N6" s="86"/>
-      <c r="O6" s="86"/>
-      <c r="P6" s="86"/>
-      <c r="Q6" s="86"/>
-      <c r="R6" s="86"/>
-      <c r="S6" s="86"/>
-      <c r="T6" s="86"/>
-      <c r="U6" s="86"/>
-      <c r="V6" s="86"/>
-      <c r="W6" s="86"/>
+      <c r="C6" s="121"/>
+      <c r="D6" s="121"/>
+      <c r="E6" s="121"/>
+      <c r="F6" s="121"/>
+      <c r="G6" s="121"/>
+      <c r="H6" s="121"/>
+      <c r="I6" s="121"/>
+      <c r="J6" s="121"/>
+      <c r="K6" s="121"/>
+      <c r="L6" s="121"/>
+      <c r="M6" s="121"/>
+      <c r="N6" s="121"/>
+      <c r="O6" s="121"/>
+      <c r="P6" s="121"/>
+      <c r="Q6" s="121"/>
+      <c r="R6" s="121"/>
+      <c r="S6" s="121"/>
+      <c r="T6" s="121"/>
+      <c r="U6" s="121"/>
+      <c r="V6" s="121"/>
+      <c r="W6" s="121"/>
       <c r="X6" s="5"/>
       <c r="Y6" s="5"/>
       <c r="Z6" s="5"/>
@@ -2204,30 +2277,30 @@
       <c r="AK6" s="6"/>
     </row>
     <row r="7" spans="1:43" ht="26.25" customHeight="1">
-      <c r="B7" s="98" t="s">
+      <c r="B7" s="122" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="86"/>
-      <c r="D7" s="86"/>
-      <c r="E7" s="86"/>
-      <c r="F7" s="86"/>
-      <c r="G7" s="86"/>
-      <c r="H7" s="86"/>
-      <c r="I7" s="86"/>
-      <c r="J7" s="86"/>
-      <c r="K7" s="86"/>
-      <c r="L7" s="86"/>
-      <c r="M7" s="86"/>
-      <c r="N7" s="86"/>
-      <c r="O7" s="86"/>
-      <c r="P7" s="86"/>
-      <c r="Q7" s="86"/>
-      <c r="R7" s="86"/>
-      <c r="S7" s="86"/>
-      <c r="T7" s="86"/>
-      <c r="U7" s="86"/>
-      <c r="V7" s="86"/>
-      <c r="W7" s="86"/>
+      <c r="C7" s="121"/>
+      <c r="D7" s="121"/>
+      <c r="E7" s="121"/>
+      <c r="F7" s="121"/>
+      <c r="G7" s="121"/>
+      <c r="H7" s="121"/>
+      <c r="I7" s="121"/>
+      <c r="J7" s="121"/>
+      <c r="K7" s="121"/>
+      <c r="L7" s="121"/>
+      <c r="M7" s="121"/>
+      <c r="N7" s="121"/>
+      <c r="O7" s="121"/>
+      <c r="P7" s="121"/>
+      <c r="Q7" s="121"/>
+      <c r="R7" s="121"/>
+      <c r="S7" s="121"/>
+      <c r="T7" s="121"/>
+      <c r="U7" s="121"/>
+      <c r="V7" s="121"/>
+      <c r="W7" s="121"/>
       <c r="X7" s="5"/>
       <c r="Y7" s="5"/>
       <c r="Z7" s="5"/>
@@ -2244,30 +2317,30 @@
       <c r="AK7" s="6"/>
     </row>
     <row r="8" spans="1:43" ht="51" customHeight="1">
-      <c r="B8" s="122" t="s">
+      <c r="B8" s="123" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="86"/>
-      <c r="D8" s="86"/>
-      <c r="E8" s="86"/>
-      <c r="F8" s="86"/>
-      <c r="G8" s="86"/>
-      <c r="H8" s="86"/>
-      <c r="I8" s="86"/>
-      <c r="J8" s="86"/>
-      <c r="K8" s="86"/>
-      <c r="L8" s="86"/>
-      <c r="M8" s="86"/>
-      <c r="N8" s="86"/>
-      <c r="O8" s="86"/>
-      <c r="P8" s="86"/>
-      <c r="Q8" s="86"/>
-      <c r="R8" s="86"/>
-      <c r="S8" s="86"/>
-      <c r="T8" s="86"/>
-      <c r="U8" s="86"/>
-      <c r="V8" s="86"/>
-      <c r="W8" s="86"/>
+      <c r="C8" s="121"/>
+      <c r="D8" s="121"/>
+      <c r="E8" s="121"/>
+      <c r="F8" s="121"/>
+      <c r="G8" s="121"/>
+      <c r="H8" s="121"/>
+      <c r="I8" s="121"/>
+      <c r="J8" s="121"/>
+      <c r="K8" s="121"/>
+      <c r="L8" s="121"/>
+      <c r="M8" s="121"/>
+      <c r="N8" s="121"/>
+      <c r="O8" s="121"/>
+      <c r="P8" s="121"/>
+      <c r="Q8" s="121"/>
+      <c r="R8" s="121"/>
+      <c r="S8" s="121"/>
+      <c r="T8" s="121"/>
+      <c r="U8" s="121"/>
+      <c r="V8" s="121"/>
+      <c r="W8" s="121"/>
       <c r="X8" s="5"/>
       <c r="Y8" s="5"/>
       <c r="Z8" s="5"/>
@@ -2322,30 +2395,30 @@
       <c r="AK9" s="6"/>
     </row>
     <row r="10" spans="1:43" ht="20.25" customHeight="1">
-      <c r="B10" s="122" t="s">
+      <c r="B10" s="123" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="86"/>
-      <c r="D10" s="86"/>
-      <c r="E10" s="86"/>
-      <c r="F10" s="86"/>
-      <c r="G10" s="86"/>
-      <c r="H10" s="86"/>
-      <c r="I10" s="86"/>
-      <c r="J10" s="86"/>
-      <c r="K10" s="86"/>
-      <c r="L10" s="86"/>
-      <c r="M10" s="86"/>
-      <c r="N10" s="86"/>
-      <c r="O10" s="86"/>
-      <c r="P10" s="86"/>
-      <c r="Q10" s="86"/>
-      <c r="R10" s="86"/>
-      <c r="S10" s="86"/>
-      <c r="T10" s="86"/>
-      <c r="U10" s="86"/>
-      <c r="V10" s="86"/>
-      <c r="W10" s="86"/>
+      <c r="C10" s="121"/>
+      <c r="D10" s="121"/>
+      <c r="E10" s="121"/>
+      <c r="F10" s="121"/>
+      <c r="G10" s="121"/>
+      <c r="H10" s="121"/>
+      <c r="I10" s="121"/>
+      <c r="J10" s="121"/>
+      <c r="K10" s="121"/>
+      <c r="L10" s="121"/>
+      <c r="M10" s="121"/>
+      <c r="N10" s="121"/>
+      <c r="O10" s="121"/>
+      <c r="P10" s="121"/>
+      <c r="Q10" s="121"/>
+      <c r="R10" s="121"/>
+      <c r="S10" s="121"/>
+      <c r="T10" s="121"/>
+      <c r="U10" s="121"/>
+      <c r="V10" s="121"/>
+      <c r="W10" s="121"/>
       <c r="X10" s="5"/>
       <c r="Y10" s="5"/>
       <c r="Z10" s="5"/>
@@ -2363,30 +2436,30 @@
     </row>
     <row r="11" spans="1:43" ht="60" customHeight="1">
       <c r="A11" s="8"/>
-      <c r="B11" s="98" t="s">
+      <c r="B11" s="122" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="86"/>
-      <c r="D11" s="86"/>
-      <c r="E11" s="86"/>
-      <c r="F11" s="86"/>
-      <c r="G11" s="86"/>
-      <c r="H11" s="86"/>
-      <c r="I11" s="86"/>
-      <c r="J11" s="86"/>
-      <c r="K11" s="86"/>
-      <c r="L11" s="86"/>
-      <c r="M11" s="86"/>
-      <c r="N11" s="86"/>
-      <c r="O11" s="86"/>
-      <c r="P11" s="86"/>
-      <c r="Q11" s="86"/>
-      <c r="R11" s="86"/>
-      <c r="S11" s="86"/>
-      <c r="T11" s="86"/>
-      <c r="U11" s="86"/>
-      <c r="V11" s="86"/>
-      <c r="W11" s="86"/>
+      <c r="C11" s="121"/>
+      <c r="D11" s="121"/>
+      <c r="E11" s="121"/>
+      <c r="F11" s="121"/>
+      <c r="G11" s="121"/>
+      <c r="H11" s="121"/>
+      <c r="I11" s="121"/>
+      <c r="J11" s="121"/>
+      <c r="K11" s="121"/>
+      <c r="L11" s="121"/>
+      <c r="M11" s="121"/>
+      <c r="N11" s="121"/>
+      <c r="O11" s="121"/>
+      <c r="P11" s="121"/>
+      <c r="Q11" s="121"/>
+      <c r="R11" s="121"/>
+      <c r="S11" s="121"/>
+      <c r="T11" s="121"/>
+      <c r="U11" s="121"/>
+      <c r="V11" s="121"/>
+      <c r="W11" s="121"/>
       <c r="X11" s="9"/>
       <c r="Y11" s="9"/>
       <c r="Z11" s="9"/>
@@ -2409,30 +2482,30 @@
       <c r="AQ11" s="8"/>
     </row>
     <row r="12" spans="1:43" ht="20.25" customHeight="1">
-      <c r="B12" s="98" t="s">
+      <c r="B12" s="122" t="s">
         <v>10</v>
       </c>
-      <c r="C12" s="86"/>
-      <c r="D12" s="86"/>
-      <c r="E12" s="86"/>
-      <c r="F12" s="86"/>
-      <c r="G12" s="86"/>
-      <c r="H12" s="86"/>
-      <c r="I12" s="86"/>
-      <c r="J12" s="86"/>
-      <c r="K12" s="86"/>
-      <c r="L12" s="86"/>
-      <c r="M12" s="86"/>
-      <c r="N12" s="86"/>
-      <c r="O12" s="86"/>
-      <c r="P12" s="86"/>
-      <c r="Q12" s="86"/>
-      <c r="R12" s="86"/>
-      <c r="S12" s="86"/>
-      <c r="T12" s="86"/>
-      <c r="U12" s="86"/>
-      <c r="V12" s="86"/>
-      <c r="W12" s="86"/>
+      <c r="C12" s="121"/>
+      <c r="D12" s="121"/>
+      <c r="E12" s="121"/>
+      <c r="F12" s="121"/>
+      <c r="G12" s="121"/>
+      <c r="H12" s="121"/>
+      <c r="I12" s="121"/>
+      <c r="J12" s="121"/>
+      <c r="K12" s="121"/>
+      <c r="L12" s="121"/>
+      <c r="M12" s="121"/>
+      <c r="N12" s="121"/>
+      <c r="O12" s="121"/>
+      <c r="P12" s="121"/>
+      <c r="Q12" s="121"/>
+      <c r="R12" s="121"/>
+      <c r="S12" s="121"/>
+      <c r="T12" s="121"/>
+      <c r="U12" s="121"/>
+      <c r="V12" s="121"/>
+      <c r="W12" s="121"/>
       <c r="X12" s="5"/>
       <c r="Y12" s="5"/>
       <c r="Z12" s="5"/>
@@ -2449,30 +2522,30 @@
       <c r="AK12" s="6"/>
     </row>
     <row r="13" spans="1:43" ht="20.25" customHeight="1">
-      <c r="B13" s="98" t="s">
+      <c r="B13" s="122" t="s">
         <v>11</v>
       </c>
-      <c r="C13" s="86"/>
-      <c r="D13" s="86"/>
-      <c r="E13" s="86"/>
-      <c r="F13" s="86"/>
-      <c r="G13" s="86"/>
-      <c r="H13" s="86"/>
-      <c r="I13" s="86"/>
-      <c r="J13" s="86"/>
-      <c r="K13" s="86"/>
-      <c r="L13" s="86"/>
-      <c r="M13" s="86"/>
-      <c r="N13" s="86"/>
-      <c r="O13" s="86"/>
-      <c r="P13" s="86"/>
-      <c r="Q13" s="86"/>
-      <c r="R13" s="86"/>
-      <c r="S13" s="86"/>
-      <c r="T13" s="86"/>
-      <c r="U13" s="86"/>
-      <c r="V13" s="86"/>
-      <c r="W13" s="86"/>
+      <c r="C13" s="121"/>
+      <c r="D13" s="121"/>
+      <c r="E13" s="121"/>
+      <c r="F13" s="121"/>
+      <c r="G13" s="121"/>
+      <c r="H13" s="121"/>
+      <c r="I13" s="121"/>
+      <c r="J13" s="121"/>
+      <c r="K13" s="121"/>
+      <c r="L13" s="121"/>
+      <c r="M13" s="121"/>
+      <c r="N13" s="121"/>
+      <c r="O13" s="121"/>
+      <c r="P13" s="121"/>
+      <c r="Q13" s="121"/>
+      <c r="R13" s="121"/>
+      <c r="S13" s="121"/>
+      <c r="T13" s="121"/>
+      <c r="U13" s="121"/>
+      <c r="V13" s="121"/>
+      <c r="W13" s="121"/>
       <c r="X13" s="5"/>
       <c r="Y13" s="5"/>
       <c r="Z13" s="5"/>
@@ -2527,30 +2600,30 @@
       <c r="AK14" s="6"/>
     </row>
     <row r="15" spans="1:43" ht="24.75" customHeight="1">
-      <c r="B15" s="99" t="s">
+      <c r="B15" s="124" t="s">
         <v>12</v>
       </c>
-      <c r="C15" s="86"/>
-      <c r="D15" s="86"/>
-      <c r="E15" s="86"/>
-      <c r="F15" s="86"/>
-      <c r="G15" s="86"/>
-      <c r="H15" s="86"/>
-      <c r="I15" s="86"/>
-      <c r="J15" s="86"/>
-      <c r="K15" s="86"/>
-      <c r="L15" s="86"/>
-      <c r="M15" s="86"/>
-      <c r="N15" s="86"/>
-      <c r="O15" s="86"/>
-      <c r="P15" s="86"/>
-      <c r="Q15" s="86"/>
-      <c r="R15" s="86"/>
-      <c r="S15" s="86"/>
-      <c r="T15" s="86"/>
-      <c r="U15" s="86"/>
-      <c r="V15" s="86"/>
-      <c r="W15" s="86"/>
+      <c r="C15" s="121"/>
+      <c r="D15" s="121"/>
+      <c r="E15" s="121"/>
+      <c r="F15" s="121"/>
+      <c r="G15" s="121"/>
+      <c r="H15" s="121"/>
+      <c r="I15" s="121"/>
+      <c r="J15" s="121"/>
+      <c r="K15" s="121"/>
+      <c r="L15" s="121"/>
+      <c r="M15" s="121"/>
+      <c r="N15" s="121"/>
+      <c r="O15" s="121"/>
+      <c r="P15" s="121"/>
+      <c r="Q15" s="121"/>
+      <c r="R15" s="121"/>
+      <c r="S15" s="121"/>
+      <c r="T15" s="121"/>
+      <c r="U15" s="121"/>
+      <c r="V15" s="121"/>
+      <c r="W15" s="121"/>
       <c r="X15" s="5"/>
       <c r="Y15" s="5"/>
       <c r="Z15" s="5"/>
@@ -2568,30 +2641,30 @@
     </row>
     <row r="16" spans="1:43" ht="24.75" customHeight="1">
       <c r="A16" s="2"/>
-      <c r="B16" s="100" t="s">
+      <c r="B16" s="125" t="s">
         <v>13</v>
       </c>
-      <c r="C16" s="86"/>
-      <c r="D16" s="86"/>
-      <c r="E16" s="86"/>
-      <c r="F16" s="86"/>
-      <c r="G16" s="86"/>
-      <c r="H16" s="86"/>
-      <c r="I16" s="86"/>
-      <c r="J16" s="86"/>
-      <c r="K16" s="86"/>
-      <c r="L16" s="86"/>
-      <c r="M16" s="86"/>
-      <c r="N16" s="86"/>
-      <c r="O16" s="86"/>
-      <c r="P16" s="86"/>
-      <c r="Q16" s="86"/>
-      <c r="R16" s="86"/>
-      <c r="S16" s="86"/>
-      <c r="T16" s="86"/>
-      <c r="U16" s="86"/>
-      <c r="V16" s="86"/>
-      <c r="W16" s="86"/>
+      <c r="C16" s="121"/>
+      <c r="D16" s="121"/>
+      <c r="E16" s="121"/>
+      <c r="F16" s="121"/>
+      <c r="G16" s="121"/>
+      <c r="H16" s="121"/>
+      <c r="I16" s="121"/>
+      <c r="J16" s="121"/>
+      <c r="K16" s="121"/>
+      <c r="L16" s="121"/>
+      <c r="M16" s="121"/>
+      <c r="N16" s="121"/>
+      <c r="O16" s="121"/>
+      <c r="P16" s="121"/>
+      <c r="Q16" s="121"/>
+      <c r="R16" s="121"/>
+      <c r="S16" s="121"/>
+      <c r="T16" s="121"/>
+      <c r="U16" s="121"/>
+      <c r="V16" s="121"/>
+      <c r="W16" s="121"/>
       <c r="X16" s="12"/>
       <c r="Y16" s="12"/>
       <c r="Z16" s="12"/>
@@ -2614,30 +2687,30 @@
       <c r="AQ16" s="2"/>
     </row>
     <row r="17" spans="1:43" ht="24.75" customHeight="1">
-      <c r="B17" s="99" t="s">
+      <c r="B17" s="124" t="s">
         <v>14</v>
       </c>
-      <c r="C17" s="86"/>
-      <c r="D17" s="86"/>
-      <c r="E17" s="86"/>
-      <c r="F17" s="86"/>
-      <c r="G17" s="86"/>
-      <c r="H17" s="86"/>
-      <c r="I17" s="86"/>
-      <c r="J17" s="86"/>
-      <c r="K17" s="86"/>
-      <c r="L17" s="86"/>
-      <c r="M17" s="86"/>
-      <c r="N17" s="86"/>
-      <c r="O17" s="86"/>
-      <c r="P17" s="86"/>
-      <c r="Q17" s="86"/>
-      <c r="R17" s="86"/>
-      <c r="S17" s="86"/>
-      <c r="T17" s="86"/>
-      <c r="U17" s="86"/>
-      <c r="V17" s="86"/>
-      <c r="W17" s="86"/>
+      <c r="C17" s="121"/>
+      <c r="D17" s="121"/>
+      <c r="E17" s="121"/>
+      <c r="F17" s="121"/>
+      <c r="G17" s="121"/>
+      <c r="H17" s="121"/>
+      <c r="I17" s="121"/>
+      <c r="J17" s="121"/>
+      <c r="K17" s="121"/>
+      <c r="L17" s="121"/>
+      <c r="M17" s="121"/>
+      <c r="N17" s="121"/>
+      <c r="O17" s="121"/>
+      <c r="P17" s="121"/>
+      <c r="Q17" s="121"/>
+      <c r="R17" s="121"/>
+      <c r="S17" s="121"/>
+      <c r="T17" s="121"/>
+      <c r="U17" s="121"/>
+      <c r="V17" s="121"/>
+      <c r="W17" s="121"/>
       <c r="X17" s="5"/>
       <c r="Y17" s="5"/>
       <c r="Z17" s="5"/>
@@ -2654,28 +2727,28 @@
       <c r="AK17" s="6"/>
     </row>
     <row r="18" spans="1:43" ht="6.75" customHeight="1">
-      <c r="B18" s="99"/>
-      <c r="C18" s="86"/>
-      <c r="D18" s="86"/>
-      <c r="E18" s="86"/>
-      <c r="F18" s="86"/>
-      <c r="G18" s="86"/>
-      <c r="H18" s="86"/>
-      <c r="I18" s="86"/>
-      <c r="J18" s="86"/>
-      <c r="K18" s="86"/>
-      <c r="L18" s="86"/>
-      <c r="M18" s="86"/>
-      <c r="N18" s="86"/>
-      <c r="O18" s="86"/>
-      <c r="P18" s="86"/>
-      <c r="Q18" s="86"/>
-      <c r="R18" s="86"/>
-      <c r="S18" s="86"/>
-      <c r="T18" s="86"/>
-      <c r="U18" s="86"/>
-      <c r="V18" s="86"/>
-      <c r="W18" s="86"/>
+      <c r="B18" s="124"/>
+      <c r="C18" s="121"/>
+      <c r="D18" s="121"/>
+      <c r="E18" s="121"/>
+      <c r="F18" s="121"/>
+      <c r="G18" s="121"/>
+      <c r="H18" s="121"/>
+      <c r="I18" s="121"/>
+      <c r="J18" s="121"/>
+      <c r="K18" s="121"/>
+      <c r="L18" s="121"/>
+      <c r="M18" s="121"/>
+      <c r="N18" s="121"/>
+      <c r="O18" s="121"/>
+      <c r="P18" s="121"/>
+      <c r="Q18" s="121"/>
+      <c r="R18" s="121"/>
+      <c r="S18" s="121"/>
+      <c r="T18" s="121"/>
+      <c r="U18" s="121"/>
+      <c r="V18" s="121"/>
+      <c r="W18" s="121"/>
       <c r="X18" s="5"/>
       <c r="Y18" s="5"/>
       <c r="Z18" s="5"/>
@@ -2693,38 +2766,38 @@
     </row>
     <row r="19" spans="1:43" ht="10.5" customHeight="1">
       <c r="A19" s="14"/>
-      <c r="B19" s="107" t="s">
+      <c r="B19" s="129" t="s">
         <v>15</v>
       </c>
-      <c r="C19" s="140" t="s">
+      <c r="C19" s="142" t="s">
         <v>16</v>
       </c>
-      <c r="D19" s="102"/>
-      <c r="E19" s="103"/>
-      <c r="F19" s="110" t="s">
+      <c r="D19" s="127"/>
+      <c r="E19" s="128"/>
+      <c r="F19" s="132" t="s">
         <v>17</v>
       </c>
-      <c r="G19" s="101" t="s">
+      <c r="G19" s="126" t="s">
         <v>18</v>
       </c>
-      <c r="H19" s="102"/>
-      <c r="I19" s="102"/>
-      <c r="J19" s="103"/>
-      <c r="K19" s="101" t="s">
+      <c r="H19" s="127"/>
+      <c r="I19" s="127"/>
+      <c r="J19" s="128"/>
+      <c r="K19" s="126" t="s">
         <v>19</v>
       </c>
-      <c r="L19" s="102"/>
-      <c r="M19" s="102"/>
-      <c r="N19" s="102"/>
-      <c r="O19" s="102"/>
-      <c r="P19" s="102"/>
-      <c r="Q19" s="102"/>
-      <c r="R19" s="103"/>
-      <c r="S19" s="113"/>
-      <c r="T19" s="102"/>
-      <c r="U19" s="102"/>
-      <c r="V19" s="103"/>
-      <c r="W19" s="116" t="s">
+      <c r="L19" s="127"/>
+      <c r="M19" s="127"/>
+      <c r="N19" s="127"/>
+      <c r="O19" s="127"/>
+      <c r="P19" s="127"/>
+      <c r="Q19" s="127"/>
+      <c r="R19" s="128"/>
+      <c r="S19" s="135"/>
+      <c r="T19" s="127"/>
+      <c r="U19" s="127"/>
+      <c r="V19" s="128"/>
+      <c r="W19" s="138" t="s">
         <v>20</v>
       </c>
       <c r="X19" s="14"/>
@@ -2750,28 +2823,28 @@
     </row>
     <row r="20" spans="1:43" ht="10.5" customHeight="1">
       <c r="A20" s="14"/>
-      <c r="B20" s="108"/>
-      <c r="C20" s="114"/>
-      <c r="D20" s="86"/>
-      <c r="E20" s="115"/>
-      <c r="F20" s="111"/>
-      <c r="G20" s="104"/>
-      <c r="H20" s="105"/>
-      <c r="I20" s="105"/>
+      <c r="B20" s="130"/>
+      <c r="C20" s="136"/>
+      <c r="D20" s="121"/>
+      <c r="E20" s="137"/>
+      <c r="F20" s="133"/>
+      <c r="G20" s="110"/>
+      <c r="H20" s="89"/>
+      <c r="I20" s="89"/>
       <c r="J20" s="106"/>
-      <c r="K20" s="104"/>
-      <c r="L20" s="105"/>
-      <c r="M20" s="105"/>
-      <c r="N20" s="105"/>
-      <c r="O20" s="105"/>
-      <c r="P20" s="105"/>
-      <c r="Q20" s="105"/>
+      <c r="K20" s="110"/>
+      <c r="L20" s="89"/>
+      <c r="M20" s="89"/>
+      <c r="N20" s="89"/>
+      <c r="O20" s="89"/>
+      <c r="P20" s="89"/>
+      <c r="Q20" s="89"/>
       <c r="R20" s="106"/>
-      <c r="S20" s="114"/>
-      <c r="T20" s="86"/>
-      <c r="U20" s="86"/>
-      <c r="V20" s="115"/>
-      <c r="W20" s="117"/>
+      <c r="S20" s="136"/>
+      <c r="T20" s="121"/>
+      <c r="U20" s="121"/>
+      <c r="V20" s="137"/>
+      <c r="W20" s="139"/>
       <c r="X20" s="14"/>
       <c r="Y20" s="14"/>
       <c r="Z20" s="14"/>
@@ -2795,40 +2868,40 @@
     </row>
     <row r="21" spans="1:43" ht="34.5" customHeight="1">
       <c r="A21" s="15"/>
-      <c r="B21" s="108"/>
-      <c r="C21" s="114"/>
-      <c r="D21" s="86"/>
-      <c r="E21" s="115"/>
-      <c r="F21" s="111"/>
-      <c r="G21" s="139" t="s">
+      <c r="B21" s="130"/>
+      <c r="C21" s="136"/>
+      <c r="D21" s="121"/>
+      <c r="E21" s="137"/>
+      <c r="F21" s="133"/>
+      <c r="G21" s="108" t="s">
         <v>21</v>
       </c>
-      <c r="H21" s="121"/>
-      <c r="I21" s="139" t="s">
+      <c r="H21" s="85"/>
+      <c r="I21" s="108" t="s">
         <v>22</v>
       </c>
-      <c r="J21" s="121"/>
-      <c r="K21" s="139" t="s">
+      <c r="J21" s="85"/>
+      <c r="K21" s="108" t="s">
         <v>21</v>
       </c>
-      <c r="L21" s="121"/>
-      <c r="M21" s="139" t="s">
+      <c r="L21" s="85"/>
+      <c r="M21" s="108" t="s">
         <v>22</v>
       </c>
-      <c r="N21" s="121"/>
-      <c r="O21" s="137" t="s">
+      <c r="N21" s="85"/>
+      <c r="O21" s="104" t="s">
         <v>23</v>
       </c>
-      <c r="P21" s="121"/>
-      <c r="Q21" s="138" t="s">
+      <c r="P21" s="85"/>
+      <c r="Q21" s="105" t="s">
         <v>24</v>
       </c>
       <c r="R21" s="106"/>
-      <c r="S21" s="104"/>
-      <c r="T21" s="105"/>
-      <c r="U21" s="105"/>
+      <c r="S21" s="110"/>
+      <c r="T21" s="89"/>
+      <c r="U21" s="89"/>
       <c r="V21" s="106"/>
-      <c r="W21" s="117"/>
+      <c r="W21" s="139"/>
       <c r="X21" s="15"/>
       <c r="Y21" s="15"/>
       <c r="Z21" s="15"/>
@@ -2852,11 +2925,11 @@
     </row>
     <row r="22" spans="1:43" ht="38.25" customHeight="1">
       <c r="A22" s="14"/>
-      <c r="B22" s="109"/>
-      <c r="C22" s="104"/>
-      <c r="D22" s="105"/>
+      <c r="B22" s="131"/>
+      <c r="C22" s="110"/>
+      <c r="D22" s="89"/>
       <c r="E22" s="106"/>
-      <c r="F22" s="112"/>
+      <c r="F22" s="134"/>
       <c r="G22" s="16" t="s">
         <v>25</v>
       </c>
@@ -2893,11 +2966,11 @@
       <c r="R22" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="S22" s="119"/>
-      <c r="T22" s="120"/>
-      <c r="U22" s="120"/>
-      <c r="V22" s="121"/>
-      <c r="W22" s="118"/>
+      <c r="S22" s="141"/>
+      <c r="T22" s="84"/>
+      <c r="U22" s="84"/>
+      <c r="V22" s="85"/>
+      <c r="W22" s="140"/>
       <c r="X22" s="14"/>
       <c r="Y22" s="14"/>
       <c r="Z22" s="14"/>
@@ -2924,11 +2997,11 @@
       <c r="B23" s="18">
         <v>1</v>
       </c>
-      <c r="C23" s="134" t="s">
+      <c r="C23" s="93" t="s">
         <v>37</v>
       </c>
-      <c r="D23" s="129"/>
-      <c r="E23" s="130"/>
+      <c r="D23" s="87"/>
+      <c r="E23" s="94"/>
       <c r="F23" s="19">
         <v>1</v>
       </c>
@@ -2946,12 +3019,12 @@
       <c r="P23" s="22"/>
       <c r="Q23" s="22"/>
       <c r="R23" s="22"/>
-      <c r="S23" s="92" t="s">
+      <c r="S23" s="107" t="s">
         <v>39</v>
       </c>
-      <c r="T23" s="120"/>
-      <c r="U23" s="120"/>
-      <c r="V23" s="121"/>
+      <c r="T23" s="84"/>
+      <c r="U23" s="84"/>
+      <c r="V23" s="85"/>
       <c r="W23" s="23" t="s">
         <v>40</v>
       </c>
@@ -2976,61 +3049,61 @@
       <c r="AP23" s="17"/>
       <c r="AQ23" s="17"/>
     </row>
-    <row r="24" spans="1:43" s="83" customFormat="1" ht="75" customHeight="1">
-      <c r="A24" s="84"/>
-      <c r="B24" s="155"/>
-      <c r="C24" s="156"/>
-      <c r="D24" s="156"/>
-      <c r="E24" s="156"/>
-      <c r="F24" s="156"/>
-      <c r="G24" s="156"/>
-      <c r="H24" s="156"/>
-      <c r="I24" s="156"/>
-      <c r="J24" s="156"/>
-      <c r="K24" s="156"/>
-      <c r="L24" s="156"/>
-      <c r="M24" s="156"/>
-      <c r="N24" s="156"/>
-      <c r="O24" s="156"/>
-      <c r="P24" s="156"/>
-      <c r="Q24" s="156"/>
-      <c r="R24" s="156"/>
-      <c r="S24" s="156"/>
-      <c r="T24" s="156"/>
-      <c r="U24" s="156"/>
-      <c r="V24" s="156"/>
-      <c r="W24" s="157"/>
-      <c r="X24" s="84"/>
-      <c r="Y24" s="84"/>
-      <c r="Z24" s="84"/>
-      <c r="AA24" s="84"/>
-      <c r="AB24" s="84"/>
-      <c r="AC24" s="84"/>
-      <c r="AD24" s="84"/>
-      <c r="AE24" s="84"/>
-      <c r="AF24" s="84"/>
-      <c r="AG24" s="84"/>
-      <c r="AH24" s="84"/>
-      <c r="AI24" s="84"/>
-      <c r="AJ24" s="84"/>
+    <row r="24" spans="1:43" ht="75" customHeight="1">
+      <c r="A24" s="17"/>
+      <c r="B24" s="97"/>
+      <c r="C24" s="98"/>
+      <c r="D24" s="98"/>
+      <c r="E24" s="98"/>
+      <c r="F24" s="98"/>
+      <c r="G24" s="98"/>
+      <c r="H24" s="98"/>
+      <c r="I24" s="98"/>
+      <c r="J24" s="98"/>
+      <c r="K24" s="98"/>
+      <c r="L24" s="98"/>
+      <c r="M24" s="98"/>
+      <c r="N24" s="98"/>
+      <c r="O24" s="98"/>
+      <c r="P24" s="98"/>
+      <c r="Q24" s="98"/>
+      <c r="R24" s="98"/>
+      <c r="S24" s="98"/>
+      <c r="T24" s="98"/>
+      <c r="U24" s="98"/>
+      <c r="V24" s="98"/>
+      <c r="W24" s="99"/>
+      <c r="X24" s="17"/>
+      <c r="Y24" s="17"/>
+      <c r="Z24" s="17"/>
+      <c r="AA24" s="17"/>
+      <c r="AB24" s="17"/>
+      <c r="AC24" s="17"/>
+      <c r="AD24" s="17"/>
+      <c r="AE24" s="17"/>
+      <c r="AF24" s="17"/>
+      <c r="AG24" s="17"/>
+      <c r="AH24" s="17"/>
+      <c r="AI24" s="17"/>
+      <c r="AJ24" s="17"/>
       <c r="AK24" s="24"/>
-      <c r="AL24" s="84"/>
-      <c r="AM24" s="84"/>
-      <c r="AN24" s="84"/>
-      <c r="AO24" s="84"/>
-      <c r="AP24" s="84"/>
-      <c r="AQ24" s="84"/>
+      <c r="AL24" s="17"/>
+      <c r="AM24" s="17"/>
+      <c r="AN24" s="17"/>
+      <c r="AO24" s="17"/>
+      <c r="AP24" s="17"/>
+      <c r="AQ24" s="17"/>
     </row>
     <row r="25" spans="1:43" ht="239.25" customHeight="1">
       <c r="A25" s="17"/>
       <c r="B25" s="18">
         <v>2</v>
       </c>
-      <c r="C25" s="141" t="s">
+      <c r="C25" s="95" t="s">
         <v>81</v>
       </c>
-      <c r="D25" s="129"/>
-      <c r="E25" s="130"/>
+      <c r="D25" s="87"/>
+      <c r="E25" s="94"/>
       <c r="F25" s="19">
         <v>2</v>
       </c>
@@ -3048,12 +3121,12 @@
       <c r="P25" s="22"/>
       <c r="Q25" s="22"/>
       <c r="R25" s="22"/>
-      <c r="S25" s="92" t="s">
+      <c r="S25" s="107" t="s">
         <v>82</v>
       </c>
-      <c r="T25" s="120"/>
-      <c r="U25" s="120"/>
-      <c r="V25" s="121"/>
+      <c r="T25" s="84"/>
+      <c r="U25" s="84"/>
+      <c r="V25" s="85"/>
       <c r="W25" s="23" t="s">
         <v>41</v>
       </c>
@@ -3078,16 +3151,16 @@
       <c r="AP25" s="17"/>
       <c r="AQ25" s="17"/>
     </row>
-    <row r="26" spans="1:43" s="83" customFormat="1" ht="239.25" customHeight="1">
-      <c r="A26" s="84"/>
+    <row r="26" spans="1:43" ht="239.25" customHeight="1">
+      <c r="A26" s="17"/>
       <c r="B26" s="18">
         <v>3</v>
       </c>
-      <c r="C26" s="89" t="s">
+      <c r="C26" s="90" t="s">
         <v>83</v>
       </c>
-      <c r="D26" s="90"/>
-      <c r="E26" s="91"/>
+      <c r="D26" s="91"/>
+      <c r="E26" s="92"/>
       <c r="F26" s="19"/>
       <c r="G26" s="21"/>
       <c r="H26" s="21"/>
@@ -3101,46 +3174,46 @@
       <c r="P26" s="22"/>
       <c r="Q26" s="22"/>
       <c r="R26" s="22"/>
-      <c r="S26" s="95" t="s">
+      <c r="S26" s="100" t="s">
         <v>84</v>
       </c>
-      <c r="T26" s="96"/>
-      <c r="U26" s="96"/>
-      <c r="V26" s="97"/>
+      <c r="T26" s="101"/>
+      <c r="U26" s="101"/>
+      <c r="V26" s="102"/>
       <c r="W26" s="23" t="s">
         <v>78</v>
       </c>
-      <c r="X26" s="84"/>
-      <c r="Y26" s="84"/>
-      <c r="Z26" s="84"/>
-      <c r="AA26" s="84"/>
-      <c r="AB26" s="84"/>
-      <c r="AC26" s="84"/>
-      <c r="AD26" s="84"/>
-      <c r="AE26" s="84"/>
-      <c r="AF26" s="84"/>
-      <c r="AG26" s="84"/>
-      <c r="AH26" s="84"/>
-      <c r="AI26" s="84"/>
-      <c r="AJ26" s="84"/>
-      <c r="AK26" s="84"/>
-      <c r="AL26" s="84"/>
-      <c r="AM26" s="84"/>
-      <c r="AN26" s="84"/>
-      <c r="AO26" s="84"/>
-      <c r="AP26" s="84"/>
-      <c r="AQ26" s="84"/>
+      <c r="X26" s="17"/>
+      <c r="Y26" s="17"/>
+      <c r="Z26" s="17"/>
+      <c r="AA26" s="17"/>
+      <c r="AB26" s="17"/>
+      <c r="AC26" s="17"/>
+      <c r="AD26" s="17"/>
+      <c r="AE26" s="17"/>
+      <c r="AF26" s="17"/>
+      <c r="AG26" s="17"/>
+      <c r="AH26" s="17"/>
+      <c r="AI26" s="17"/>
+      <c r="AJ26" s="17"/>
+      <c r="AK26" s="17"/>
+      <c r="AL26" s="17"/>
+      <c r="AM26" s="17"/>
+      <c r="AN26" s="17"/>
+      <c r="AO26" s="17"/>
+      <c r="AP26" s="17"/>
+      <c r="AQ26" s="17"/>
     </row>
     <row r="27" spans="1:43" ht="239.25" customHeight="1">
       <c r="A27" s="17"/>
       <c r="B27" s="18">
         <v>3</v>
       </c>
-      <c r="C27" s="89" t="s">
+      <c r="C27" s="90" t="s">
         <v>85</v>
       </c>
-      <c r="D27" s="90"/>
-      <c r="E27" s="91"/>
+      <c r="D27" s="91"/>
+      <c r="E27" s="92"/>
       <c r="F27" s="19">
         <v>3</v>
       </c>
@@ -3158,12 +3231,12 @@
       <c r="P27" s="22"/>
       <c r="Q27" s="22"/>
       <c r="R27" s="22"/>
-      <c r="S27" s="92" t="s">
+      <c r="S27" s="107" t="s">
         <v>86</v>
       </c>
-      <c r="T27" s="93"/>
-      <c r="U27" s="93"/>
-      <c r="V27" s="94"/>
+      <c r="T27" s="146"/>
+      <c r="U27" s="146"/>
+      <c r="V27" s="147"/>
       <c r="W27" s="23" t="s">
         <v>41</v>
       </c>
@@ -3193,11 +3266,11 @@
       <c r="B28" s="18">
         <v>4</v>
       </c>
-      <c r="C28" s="89" t="s">
+      <c r="C28" s="90" t="s">
         <v>87</v>
       </c>
-      <c r="D28" s="90"/>
-      <c r="E28" s="91"/>
+      <c r="D28" s="91"/>
+      <c r="E28" s="92"/>
       <c r="F28" s="19">
         <v>4</v>
       </c>
@@ -3215,12 +3288,12 @@
       <c r="P28" s="22"/>
       <c r="Q28" s="22"/>
       <c r="R28" s="22"/>
-      <c r="S28" s="92" t="s">
+      <c r="S28" s="107" t="s">
         <v>88</v>
       </c>
-      <c r="T28" s="93"/>
-      <c r="U28" s="93"/>
-      <c r="V28" s="94"/>
+      <c r="T28" s="146"/>
+      <c r="U28" s="146"/>
+      <c r="V28" s="147"/>
       <c r="W28" s="23" t="s">
         <v>40</v>
       </c>
@@ -3250,11 +3323,11 @@
       <c r="B29" s="18">
         <v>5</v>
       </c>
-      <c r="C29" s="89" t="s">
+      <c r="C29" s="90" t="s">
         <v>89</v>
       </c>
-      <c r="D29" s="90"/>
-      <c r="E29" s="91"/>
+      <c r="D29" s="91"/>
+      <c r="E29" s="92"/>
       <c r="F29" s="19">
         <v>5</v>
       </c>
@@ -3272,12 +3345,12 @@
       <c r="P29" s="22"/>
       <c r="Q29" s="22"/>
       <c r="R29" s="22"/>
-      <c r="S29" s="95" t="s">
+      <c r="S29" s="100" t="s">
         <v>90</v>
       </c>
-      <c r="T29" s="96"/>
-      <c r="U29" s="96"/>
-      <c r="V29" s="97"/>
+      <c r="T29" s="101"/>
+      <c r="U29" s="101"/>
+      <c r="V29" s="102"/>
       <c r="W29" s="23" t="s">
         <v>78</v>
       </c>
@@ -3307,11 +3380,11 @@
       <c r="B30" s="18">
         <v>6</v>
       </c>
-      <c r="C30" s="89" t="s">
+      <c r="C30" s="90" t="s">
         <v>91</v>
       </c>
-      <c r="D30" s="90"/>
-      <c r="E30" s="91"/>
+      <c r="D30" s="91"/>
+      <c r="E30" s="92"/>
       <c r="F30" s="19">
         <v>6</v>
       </c>
@@ -3329,12 +3402,12 @@
       <c r="P30" s="22"/>
       <c r="Q30" s="22"/>
       <c r="R30" s="22"/>
-      <c r="S30" s="95" t="s">
+      <c r="S30" s="100" t="s">
         <v>92</v>
       </c>
-      <c r="T30" s="96"/>
-      <c r="U30" s="96"/>
-      <c r="V30" s="97"/>
+      <c r="T30" s="101"/>
+      <c r="U30" s="101"/>
+      <c r="V30" s="102"/>
       <c r="W30" s="23" t="s">
         <v>41</v>
       </c>
@@ -3364,11 +3437,11 @@
       <c r="B31" s="18">
         <v>7</v>
       </c>
-      <c r="C31" s="134" t="s">
+      <c r="C31" s="93" t="s">
         <v>42</v>
       </c>
-      <c r="D31" s="129"/>
-      <c r="E31" s="130"/>
+      <c r="D31" s="87"/>
+      <c r="E31" s="94"/>
       <c r="F31" s="19">
         <v>7</v>
       </c>
@@ -3386,12 +3459,12 @@
       <c r="P31" s="22"/>
       <c r="Q31" s="22"/>
       <c r="R31" s="22"/>
-      <c r="S31" s="92" t="s">
+      <c r="S31" s="107" t="s">
         <v>43</v>
       </c>
-      <c r="T31" s="120"/>
-      <c r="U31" s="120"/>
-      <c r="V31" s="121"/>
+      <c r="T31" s="84"/>
+      <c r="U31" s="84"/>
+      <c r="V31" s="85"/>
       <c r="W31" s="23" t="s">
         <v>41</v>
       </c>
@@ -3421,11 +3494,11 @@
       <c r="B32" s="18">
         <v>8</v>
       </c>
-      <c r="C32" s="134" t="s">
+      <c r="C32" s="93" t="s">
         <v>44</v>
       </c>
-      <c r="D32" s="129"/>
-      <c r="E32" s="130"/>
+      <c r="D32" s="87"/>
+      <c r="E32" s="94"/>
       <c r="F32" s="19">
         <v>8</v>
       </c>
@@ -3443,12 +3516,12 @@
       <c r="P32" s="22"/>
       <c r="Q32" s="22"/>
       <c r="R32" s="22"/>
-      <c r="S32" s="92" t="s">
+      <c r="S32" s="107" t="s">
         <v>45</v>
       </c>
-      <c r="T32" s="120"/>
-      <c r="U32" s="120"/>
-      <c r="V32" s="121"/>
+      <c r="T32" s="84"/>
+      <c r="U32" s="84"/>
+      <c r="V32" s="85"/>
       <c r="W32" s="23" t="s">
         <v>46</v>
       </c>
@@ -3478,11 +3551,11 @@
       <c r="B33" s="18">
         <v>9</v>
       </c>
-      <c r="C33" s="134" t="s">
+      <c r="C33" s="93" t="s">
         <v>47</v>
       </c>
-      <c r="D33" s="129"/>
-      <c r="E33" s="130"/>
+      <c r="D33" s="87"/>
+      <c r="E33" s="94"/>
       <c r="F33" s="27">
         <v>9</v>
       </c>
@@ -3500,12 +3573,12 @@
       </c>
       <c r="Q33" s="22"/>
       <c r="R33" s="22"/>
-      <c r="S33" s="92" t="s">
+      <c r="S33" s="107" t="s">
         <v>48</v>
       </c>
-      <c r="T33" s="120"/>
-      <c r="U33" s="120"/>
-      <c r="V33" s="121"/>
+      <c r="T33" s="84"/>
+      <c r="U33" s="84"/>
+      <c r="V33" s="85"/>
       <c r="W33" s="23" t="s">
         <v>46</v>
       </c>
@@ -3533,9 +3606,9 @@
     <row r="34" spans="1:43" ht="163.5" customHeight="1">
       <c r="A34" s="17"/>
       <c r="B34" s="18"/>
-      <c r="C34" s="134"/>
-      <c r="D34" s="129"/>
-      <c r="E34" s="130"/>
+      <c r="C34" s="93"/>
+      <c r="D34" s="87"/>
+      <c r="E34" s="94"/>
       <c r="F34" s="29"/>
       <c r="G34" s="21"/>
       <c r="H34" s="21"/>
@@ -3549,12 +3622,12 @@
       <c r="P34" s="22"/>
       <c r="Q34" s="22"/>
       <c r="R34" s="22"/>
-      <c r="S34" s="92" t="s">
+      <c r="S34" s="107" t="s">
         <v>49</v>
       </c>
-      <c r="T34" s="120"/>
-      <c r="U34" s="120"/>
-      <c r="V34" s="121"/>
+      <c r="T34" s="84"/>
+      <c r="U34" s="84"/>
+      <c r="V34" s="85"/>
       <c r="W34" s="23"/>
       <c r="X34" s="17"/>
       <c r="Y34" s="17"/>
@@ -3580,9 +3653,9 @@
     <row r="35" spans="1:43" ht="209.25" customHeight="1">
       <c r="A35" s="17"/>
       <c r="B35" s="18"/>
-      <c r="C35" s="134"/>
-      <c r="D35" s="129"/>
-      <c r="E35" s="130"/>
+      <c r="C35" s="93"/>
+      <c r="D35" s="87"/>
+      <c r="E35" s="94"/>
       <c r="F35" s="30"/>
       <c r="G35" s="21"/>
       <c r="H35" s="21"/>
@@ -3596,10 +3669,10 @@
       <c r="P35" s="22"/>
       <c r="Q35" s="22"/>
       <c r="R35" s="22"/>
-      <c r="S35" s="92"/>
-      <c r="T35" s="120"/>
-      <c r="U35" s="120"/>
-      <c r="V35" s="121"/>
+      <c r="S35" s="107"/>
+      <c r="T35" s="84"/>
+      <c r="U35" s="84"/>
+      <c r="V35" s="85"/>
       <c r="W35" s="23"/>
       <c r="X35" s="17"/>
       <c r="Y35" s="17"/>
@@ -3625,9 +3698,9 @@
     <row r="36" spans="1:43" ht="262.5" customHeight="1">
       <c r="A36" s="17"/>
       <c r="B36" s="18"/>
-      <c r="C36" s="134"/>
-      <c r="D36" s="129"/>
-      <c r="E36" s="130"/>
+      <c r="C36" s="93"/>
+      <c r="D36" s="87"/>
+      <c r="E36" s="94"/>
       <c r="F36" s="30"/>
       <c r="G36" s="21"/>
       <c r="H36" s="21"/>
@@ -3641,10 +3714,10 @@
       <c r="P36" s="22"/>
       <c r="Q36" s="22"/>
       <c r="R36" s="22"/>
-      <c r="S36" s="92"/>
-      <c r="T36" s="120"/>
-      <c r="U36" s="120"/>
-      <c r="V36" s="121"/>
+      <c r="S36" s="107"/>
+      <c r="T36" s="84"/>
+      <c r="U36" s="84"/>
+      <c r="V36" s="85"/>
       <c r="W36" s="23"/>
       <c r="X36" s="17"/>
       <c r="Y36" s="17"/>
@@ -3670,9 +3743,9 @@
     <row r="37" spans="1:43" ht="90.75" customHeight="1">
       <c r="A37" s="17"/>
       <c r="B37" s="18"/>
-      <c r="C37" s="142"/>
-      <c r="D37" s="129"/>
-      <c r="E37" s="130"/>
+      <c r="C37" s="96"/>
+      <c r="D37" s="87"/>
+      <c r="E37" s="94"/>
       <c r="F37" s="30"/>
       <c r="G37" s="21"/>
       <c r="H37" s="21"/>
@@ -3686,10 +3759,10 @@
       <c r="P37" s="22"/>
       <c r="Q37" s="22"/>
       <c r="R37" s="22"/>
-      <c r="S37" s="136"/>
-      <c r="T37" s="120"/>
-      <c r="U37" s="120"/>
-      <c r="V37" s="121"/>
+      <c r="S37" s="103"/>
+      <c r="T37" s="84"/>
+      <c r="U37" s="84"/>
+      <c r="V37" s="85"/>
       <c r="W37" s="23"/>
       <c r="X37" s="17"/>
       <c r="Y37" s="17"/>
@@ -3715,9 +3788,9 @@
     <row r="38" spans="1:43" ht="90.75" customHeight="1">
       <c r="A38" s="17"/>
       <c r="B38" s="18"/>
-      <c r="C38" s="143"/>
-      <c r="D38" s="120"/>
-      <c r="E38" s="121"/>
+      <c r="C38" s="83"/>
+      <c r="D38" s="84"/>
+      <c r="E38" s="85"/>
       <c r="F38" s="30"/>
       <c r="G38" s="21"/>
       <c r="H38" s="21"/>
@@ -3731,10 +3804,10 @@
       <c r="P38" s="22"/>
       <c r="Q38" s="22"/>
       <c r="R38" s="22"/>
-      <c r="S38" s="136"/>
-      <c r="T38" s="120"/>
-      <c r="U38" s="120"/>
-      <c r="V38" s="121"/>
+      <c r="S38" s="103"/>
+      <c r="T38" s="84"/>
+      <c r="U38" s="84"/>
+      <c r="V38" s="85"/>
       <c r="W38" s="23"/>
       <c r="X38" s="17"/>
       <c r="Y38" s="17"/>
@@ -3776,10 +3849,10 @@
       <c r="P39" s="34"/>
       <c r="Q39" s="34"/>
       <c r="R39" s="34"/>
-      <c r="S39" s="135"/>
-      <c r="T39" s="86"/>
-      <c r="U39" s="86"/>
-      <c r="V39" s="86"/>
+      <c r="S39" s="148"/>
+      <c r="T39" s="121"/>
+      <c r="U39" s="121"/>
+      <c r="V39" s="121"/>
       <c r="W39" s="35"/>
     </row>
     <row r="40" spans="1:43" ht="12.75" customHeight="1">
@@ -3801,10 +3874,10 @@
       <c r="P40" s="34"/>
       <c r="Q40" s="34"/>
       <c r="R40" s="34"/>
-      <c r="S40" s="135"/>
-      <c r="T40" s="86"/>
-      <c r="U40" s="86"/>
-      <c r="V40" s="86"/>
+      <c r="S40" s="148"/>
+      <c r="T40" s="121"/>
+      <c r="U40" s="121"/>
+      <c r="V40" s="121"/>
       <c r="W40" s="35"/>
     </row>
     <row r="41" spans="1:43" ht="19.5" customHeight="1">
@@ -3822,10 +3895,10 @@
       <c r="J41" s="17"/>
       <c r="K41" s="43"/>
       <c r="L41" s="43"/>
-      <c r="S41" s="85"/>
-      <c r="T41" s="86"/>
-      <c r="U41" s="86"/>
-      <c r="V41" s="86"/>
+      <c r="S41" s="143"/>
+      <c r="T41" s="121"/>
+      <c r="U41" s="121"/>
+      <c r="V41" s="121"/>
       <c r="W41" s="31"/>
     </row>
     <row r="42" spans="1:43" ht="18.75" customHeight="1">
@@ -3921,29 +3994,29 @@
     <row r="46" spans="1:43" ht="39.75" customHeight="1">
       <c r="A46" s="31"/>
       <c r="B46" s="32"/>
-      <c r="C46" s="87" t="s">
+      <c r="C46" s="144" t="s">
         <v>53</v>
       </c>
-      <c r="D46" s="86"/>
-      <c r="E46" s="86"/>
-      <c r="F46" s="86"/>
-      <c r="G46" s="86"/>
-      <c r="H46" s="86"/>
-      <c r="I46" s="86"/>
-      <c r="J46" s="86"/>
-      <c r="K46" s="86"/>
-      <c r="L46" s="86"/>
-      <c r="M46" s="86"/>
-      <c r="N46" s="86"/>
-      <c r="O46" s="86"/>
-      <c r="P46" s="86"/>
-      <c r="Q46" s="86"/>
-      <c r="R46" s="86"/>
-      <c r="S46" s="86"/>
-      <c r="T46" s="86"/>
-      <c r="U46" s="86"/>
-      <c r="V46" s="86"/>
-      <c r="W46" s="88"/>
+      <c r="D46" s="121"/>
+      <c r="E46" s="121"/>
+      <c r="F46" s="121"/>
+      <c r="G46" s="121"/>
+      <c r="H46" s="121"/>
+      <c r="I46" s="121"/>
+      <c r="J46" s="121"/>
+      <c r="K46" s="121"/>
+      <c r="L46" s="121"/>
+      <c r="M46" s="121"/>
+      <c r="N46" s="121"/>
+      <c r="O46" s="121"/>
+      <c r="P46" s="121"/>
+      <c r="Q46" s="121"/>
+      <c r="R46" s="121"/>
+      <c r="S46" s="121"/>
+      <c r="T46" s="121"/>
+      <c r="U46" s="121"/>
+      <c r="V46" s="121"/>
+      <c r="W46" s="145"/>
     </row>
     <row r="47" spans="1:43" ht="11.25" customHeight="1">
       <c r="A47" s="31"/>
@@ -4012,14 +4085,14 @@
       <c r="C52" s="57"/>
     </row>
     <row r="53" spans="1:13" ht="15" customHeight="1">
-      <c r="B53" s="144" t="s">
+      <c r="B53" s="86" t="s">
         <v>54</v>
       </c>
-      <c r="C53" s="129"/>
-      <c r="D53" s="129"/>
-      <c r="E53" s="129"/>
-      <c r="F53" s="129"/>
-      <c r="G53" s="129"/>
+      <c r="C53" s="87"/>
+      <c r="D53" s="87"/>
+      <c r="E53" s="87"/>
+      <c r="F53" s="87"/>
+      <c r="G53" s="87"/>
       <c r="J53" s="17"/>
     </row>
     <row r="55" spans="1:13" ht="15" customHeight="1">
@@ -4033,13 +4106,13 @@
       </c>
       <c r="D56" s="60"/>
       <c r="E56" s="60"/>
-      <c r="F56" s="145"/>
-      <c r="G56" s="105"/>
-      <c r="H56" s="105"/>
+      <c r="F56" s="88"/>
+      <c r="G56" s="89"/>
+      <c r="H56" s="89"/>
       <c r="J56" s="61"/>
-      <c r="K56" s="145"/>
-      <c r="L56" s="105"/>
-      <c r="M56" s="105"/>
+      <c r="K56" s="88"/>
+      <c r="L56" s="89"/>
+      <c r="M56" s="89"/>
     </row>
     <row r="57" spans="1:13" ht="12" customHeight="1">
       <c r="F57" s="59"/>
@@ -31313,18 +31386,52 @@
     </row>
   </sheetData>
   <mergeCells count="74">
-    <mergeCell ref="C38:E38"/>
-    <mergeCell ref="B53:G53"/>
-    <mergeCell ref="F56:H56"/>
-    <mergeCell ref="K56:M56"/>
-    <mergeCell ref="C26:E26"/>
-    <mergeCell ref="C23:E23"/>
-    <mergeCell ref="C25:E25"/>
-    <mergeCell ref="C31:E31"/>
-    <mergeCell ref="C32:E32"/>
-    <mergeCell ref="C37:E37"/>
-    <mergeCell ref="B24:W24"/>
-    <mergeCell ref="S26:V26"/>
+    <mergeCell ref="S41:V41"/>
+    <mergeCell ref="C46:W46"/>
+    <mergeCell ref="C27:E27"/>
+    <mergeCell ref="C28:E28"/>
+    <mergeCell ref="C29:E29"/>
+    <mergeCell ref="C30:E30"/>
+    <mergeCell ref="S27:V27"/>
+    <mergeCell ref="S28:V28"/>
+    <mergeCell ref="S29:V29"/>
+    <mergeCell ref="S30:V30"/>
+    <mergeCell ref="S36:V36"/>
+    <mergeCell ref="S35:V35"/>
+    <mergeCell ref="C35:E35"/>
+    <mergeCell ref="C36:E36"/>
+    <mergeCell ref="S40:V40"/>
+    <mergeCell ref="S39:V39"/>
+    <mergeCell ref="B13:W13"/>
+    <mergeCell ref="B15:W15"/>
+    <mergeCell ref="B16:W16"/>
+    <mergeCell ref="B17:W17"/>
+    <mergeCell ref="G19:J20"/>
+    <mergeCell ref="B18:W18"/>
+    <mergeCell ref="B19:B22"/>
+    <mergeCell ref="F19:F22"/>
+    <mergeCell ref="K19:R20"/>
+    <mergeCell ref="S19:V21"/>
+    <mergeCell ref="W19:W22"/>
+    <mergeCell ref="S22:V22"/>
+    <mergeCell ref="C19:E22"/>
+    <mergeCell ref="B7:W7"/>
+    <mergeCell ref="B8:W8"/>
+    <mergeCell ref="B10:W10"/>
+    <mergeCell ref="B11:W11"/>
+    <mergeCell ref="B12:W12"/>
+    <mergeCell ref="B4:F4"/>
+    <mergeCell ref="G4:M4"/>
+    <mergeCell ref="N4:T4"/>
+    <mergeCell ref="U4:W4"/>
+    <mergeCell ref="B6:W6"/>
+    <mergeCell ref="B2:F3"/>
+    <mergeCell ref="G2:M2"/>
+    <mergeCell ref="N2:T2"/>
+    <mergeCell ref="U2:W2"/>
+    <mergeCell ref="G3:M3"/>
+    <mergeCell ref="N3:T3"/>
+    <mergeCell ref="U3:W3"/>
     <mergeCell ref="S38:V38"/>
     <mergeCell ref="S37:V37"/>
     <mergeCell ref="C33:E33"/>
@@ -31341,52 +31448,18 @@
     <mergeCell ref="I21:J21"/>
     <mergeCell ref="K21:L21"/>
     <mergeCell ref="M21:N21"/>
-    <mergeCell ref="B2:F3"/>
-    <mergeCell ref="G2:M2"/>
-    <mergeCell ref="N2:T2"/>
-    <mergeCell ref="U2:W2"/>
-    <mergeCell ref="G3:M3"/>
-    <mergeCell ref="N3:T3"/>
-    <mergeCell ref="U3:W3"/>
-    <mergeCell ref="B4:F4"/>
-    <mergeCell ref="G4:M4"/>
-    <mergeCell ref="N4:T4"/>
-    <mergeCell ref="U4:W4"/>
-    <mergeCell ref="B6:W6"/>
-    <mergeCell ref="B7:W7"/>
-    <mergeCell ref="B8:W8"/>
-    <mergeCell ref="B10:W10"/>
-    <mergeCell ref="B11:W11"/>
-    <mergeCell ref="B12:W12"/>
-    <mergeCell ref="B13:W13"/>
-    <mergeCell ref="B15:W15"/>
-    <mergeCell ref="B16:W16"/>
-    <mergeCell ref="B17:W17"/>
-    <mergeCell ref="G19:J20"/>
-    <mergeCell ref="B18:W18"/>
-    <mergeCell ref="B19:B22"/>
-    <mergeCell ref="F19:F22"/>
-    <mergeCell ref="K19:R20"/>
-    <mergeCell ref="S19:V21"/>
-    <mergeCell ref="W19:W22"/>
-    <mergeCell ref="S22:V22"/>
-    <mergeCell ref="C19:E22"/>
-    <mergeCell ref="S41:V41"/>
-    <mergeCell ref="C46:W46"/>
-    <mergeCell ref="C27:E27"/>
-    <mergeCell ref="C28:E28"/>
-    <mergeCell ref="C29:E29"/>
-    <mergeCell ref="C30:E30"/>
-    <mergeCell ref="S27:V27"/>
-    <mergeCell ref="S28:V28"/>
-    <mergeCell ref="S29:V29"/>
-    <mergeCell ref="S30:V30"/>
-    <mergeCell ref="S36:V36"/>
-    <mergeCell ref="S35:V35"/>
-    <mergeCell ref="C35:E35"/>
-    <mergeCell ref="C36:E36"/>
-    <mergeCell ref="S40:V40"/>
-    <mergeCell ref="S39:V39"/>
+    <mergeCell ref="C23:E23"/>
+    <mergeCell ref="C25:E25"/>
+    <mergeCell ref="C31:E31"/>
+    <mergeCell ref="C32:E32"/>
+    <mergeCell ref="C37:E37"/>
+    <mergeCell ref="B24:W24"/>
+    <mergeCell ref="S26:V26"/>
+    <mergeCell ref="C38:E38"/>
+    <mergeCell ref="B53:G53"/>
+    <mergeCell ref="F56:H56"/>
+    <mergeCell ref="K56:M56"/>
+    <mergeCell ref="C26:E26"/>
   </mergeCells>
   <conditionalFormatting sqref="F55:G56">
     <cfRule type="cellIs" dxfId="2" priority="1" stopIfTrue="1" operator="equal">
@@ -31413,81 +31486,81 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A2:H18"/>
+  <dimension ref="A2:H31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="12.7109375" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="5" max="5" width="38.140625" customWidth="1"/>
-    <col min="6" max="6" width="22.140625" customWidth="1"/>
-    <col min="7" max="7" width="16.85546875" customWidth="1"/>
-    <col min="8" max="8" width="18.42578125" customWidth="1"/>
+    <col min="5" max="5" width="38.109375" customWidth="1"/>
+    <col min="6" max="6" width="22.109375" customWidth="1"/>
+    <col min="7" max="7" width="16.88671875" customWidth="1"/>
+    <col min="8" max="8" width="18.44140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:8" ht="15" customHeight="1">
-      <c r="A2" s="146" t="s">
+      <c r="A2" s="149" t="s">
         <v>56</v>
       </c>
-      <c r="B2" s="102"/>
-      <c r="C2" s="102"/>
-      <c r="D2" s="102"/>
-      <c r="E2" s="102"/>
-      <c r="F2" s="102"/>
-      <c r="G2" s="102"/>
-      <c r="H2" s="147"/>
+      <c r="B2" s="127"/>
+      <c r="C2" s="127"/>
+      <c r="D2" s="127"/>
+      <c r="E2" s="127"/>
+      <c r="F2" s="127"/>
+      <c r="G2" s="127"/>
+      <c r="H2" s="150"/>
     </row>
     <row r="3" spans="1:8" ht="15" customHeight="1">
-      <c r="A3" s="148"/>
-      <c r="B3" s="86"/>
-      <c r="C3" s="86"/>
-      <c r="D3" s="86"/>
-      <c r="E3" s="86"/>
-      <c r="F3" s="86"/>
-      <c r="G3" s="86"/>
-      <c r="H3" s="88"/>
+      <c r="A3" s="151"/>
+      <c r="B3" s="121"/>
+      <c r="C3" s="121"/>
+      <c r="D3" s="121"/>
+      <c r="E3" s="121"/>
+      <c r="F3" s="121"/>
+      <c r="G3" s="121"/>
+      <c r="H3" s="145"/>
     </row>
     <row r="4" spans="1:8" ht="15" customHeight="1">
-      <c r="A4" s="148"/>
-      <c r="B4" s="86"/>
-      <c r="C4" s="86"/>
-      <c r="D4" s="86"/>
-      <c r="E4" s="86"/>
-      <c r="F4" s="86"/>
-      <c r="G4" s="86"/>
-      <c r="H4" s="88"/>
+      <c r="A4" s="151"/>
+      <c r="B4" s="121"/>
+      <c r="C4" s="121"/>
+      <c r="D4" s="121"/>
+      <c r="E4" s="121"/>
+      <c r="F4" s="121"/>
+      <c r="G4" s="121"/>
+      <c r="H4" s="145"/>
     </row>
     <row r="5" spans="1:8" ht="15" customHeight="1">
-      <c r="A5" s="148"/>
-      <c r="B5" s="86"/>
-      <c r="C5" s="86"/>
-      <c r="D5" s="86"/>
-      <c r="E5" s="86"/>
-      <c r="F5" s="86"/>
-      <c r="G5" s="86"/>
-      <c r="H5" s="88"/>
+      <c r="A5" s="151"/>
+      <c r="B5" s="121"/>
+      <c r="C5" s="121"/>
+      <c r="D5" s="121"/>
+      <c r="E5" s="121"/>
+      <c r="F5" s="121"/>
+      <c r="G5" s="121"/>
+      <c r="H5" s="145"/>
     </row>
     <row r="6" spans="1:8" ht="15" customHeight="1">
-      <c r="A6" s="148"/>
-      <c r="B6" s="86"/>
-      <c r="C6" s="86"/>
-      <c r="D6" s="86"/>
-      <c r="E6" s="86"/>
-      <c r="F6" s="86"/>
-      <c r="G6" s="86"/>
-      <c r="H6" s="88"/>
+      <c r="A6" s="151"/>
+      <c r="B6" s="121"/>
+      <c r="C6" s="121"/>
+      <c r="D6" s="121"/>
+      <c r="E6" s="121"/>
+      <c r="F6" s="121"/>
+      <c r="G6" s="121"/>
+      <c r="H6" s="145"/>
     </row>
     <row r="7" spans="1:8" ht="15" customHeight="1">
-      <c r="A7" s="149"/>
-      <c r="B7" s="150"/>
-      <c r="C7" s="150"/>
-      <c r="D7" s="150"/>
-      <c r="E7" s="150"/>
-      <c r="F7" s="150"/>
-      <c r="G7" s="150"/>
-      <c r="H7" s="151"/>
+      <c r="A7" s="152"/>
+      <c r="B7" s="153"/>
+      <c r="C7" s="153"/>
+      <c r="D7" s="153"/>
+      <c r="E7" s="153"/>
+      <c r="F7" s="153"/>
+      <c r="G7" s="153"/>
+      <c r="H7" s="154"/>
     </row>
     <row r="8" spans="1:8" ht="15" customHeight="1">
       <c r="A8" s="62"/>
@@ -31520,8 +31593,8 @@
         <v>2</v>
       </c>
       <c r="F10" s="62"/>
-      <c r="G10" s="152"/>
-      <c r="H10" s="153"/>
+      <c r="G10" s="155"/>
+      <c r="H10" s="156"/>
     </row>
     <row r="11" spans="1:8" ht="15" customHeight="1">
       <c r="A11" s="62"/>
@@ -31534,8 +31607,8 @@
         <v>45278</v>
       </c>
       <c r="F11" s="62"/>
-      <c r="G11" s="86"/>
-      <c r="H11" s="86"/>
+      <c r="G11" s="121"/>
+      <c r="H11" s="121"/>
     </row>
     <row r="12" spans="1:8" ht="15" customHeight="1">
       <c r="A12" s="62" t="s">
@@ -31586,7 +31659,7 @@
       </c>
     </row>
     <row r="15" spans="1:8" ht="122.25" customHeight="1">
-      <c r="A15" s="154" t="s">
+      <c r="A15" s="157" t="s">
         <v>68</v>
       </c>
       <c r="B15" s="75">
@@ -31611,69 +31684,295 @@
         <v>73</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="141.75" customHeight="1">
-      <c r="A16" s="111"/>
+    <row r="16" spans="1:8" ht="122.25" customHeight="1">
+      <c r="A16" s="158"/>
       <c r="B16" s="75">
-        <v>45663</v>
+        <v>45643</v>
       </c>
       <c r="C16" s="76" t="s">
-        <v>69</v>
+        <v>93</v>
       </c>
       <c r="D16" s="19" t="s">
-        <v>70</v>
+        <v>94</v>
       </c>
       <c r="E16" s="77" t="s">
-        <v>74</v>
+        <v>95</v>
       </c>
       <c r="F16" s="78" t="s">
-        <v>75</v>
+        <v>41</v>
       </c>
       <c r="G16" s="79" t="s">
         <v>72</v>
       </c>
-      <c r="H16" s="80" t="s">
-        <v>76</v>
+      <c r="H16" s="78" t="s">
+        <v>96</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="165" customHeight="1">
-      <c r="A17" s="112"/>
+    <row r="17" spans="1:8" ht="122.25" customHeight="1">
+      <c r="A17" s="158"/>
       <c r="B17" s="75">
-        <v>45639</v>
+        <v>45644</v>
       </c>
       <c r="C17" s="76" t="s">
-        <v>69</v>
+        <v>97</v>
       </c>
       <c r="D17" s="19" t="s">
-        <v>70</v>
+        <v>98</v>
       </c>
       <c r="E17" s="77" t="s">
-        <v>77</v>
+        <v>99</v>
       </c>
       <c r="F17" s="78" t="s">
-        <v>78</v>
+        <v>41</v>
       </c>
       <c r="G17" s="79" t="s">
         <v>72</v>
       </c>
-      <c r="H17" s="81" t="s">
+      <c r="H17" s="78" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="122.25" customHeight="1">
+      <c r="A18" s="158"/>
+      <c r="B18" s="75">
+        <v>45645</v>
+      </c>
+      <c r="C18" s="76" t="s">
+        <v>101</v>
+      </c>
+      <c r="D18" s="19" t="s">
+        <v>102</v>
+      </c>
+      <c r="E18" s="77" t="s">
+        <v>103</v>
+      </c>
+      <c r="F18" s="78" t="s">
+        <v>41</v>
+      </c>
+      <c r="G18" s="79" t="s">
+        <v>72</v>
+      </c>
+      <c r="H18" s="78" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="141.75" customHeight="1">
+      <c r="A19" s="133"/>
+      <c r="B19" s="75">
+        <v>45663</v>
+      </c>
+      <c r="C19" s="76" t="s">
+        <v>69</v>
+      </c>
+      <c r="D19" s="19" t="s">
+        <v>70</v>
+      </c>
+      <c r="E19" s="77" t="s">
+        <v>74</v>
+      </c>
+      <c r="F19" s="78" t="s">
+        <v>75</v>
+      </c>
+      <c r="G19" s="79" t="s">
+        <v>72</v>
+      </c>
+      <c r="H19" s="80" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="165" customHeight="1">
+      <c r="A20" s="134"/>
+      <c r="B20" s="75">
+        <v>45639</v>
+      </c>
+      <c r="C20" s="76" t="s">
+        <v>69</v>
+      </c>
+      <c r="D20" s="19" t="s">
+        <v>70</v>
+      </c>
+      <c r="E20" s="77" t="s">
+        <v>77</v>
+      </c>
+      <c r="F20" s="78" t="s">
+        <v>78</v>
+      </c>
+      <c r="G20" s="79" t="s">
+        <v>72</v>
+      </c>
+      <c r="H20" s="81" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="15" customHeight="1">
-      <c r="B18" s="82"/>
-      <c r="C18" s="82"/>
-      <c r="D18" s="82"/>
-      <c r="E18" s="82"/>
-      <c r="F18" s="82"/>
-      <c r="G18" s="82"/>
-      <c r="H18" s="82"/>
+    <row r="21" spans="1:8" ht="15" customHeight="1">
+      <c r="B21" s="82"/>
+      <c r="C21" s="82"/>
+      <c r="D21" s="82"/>
+      <c r="E21" s="82"/>
+      <c r="F21" s="82"/>
+      <c r="G21" s="82"/>
+      <c r="H21" s="82"/>
+    </row>
+    <row r="24" spans="1:8" ht="15" customHeight="1">
+      <c r="A24" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" ht="15.6">
+      <c r="A26" s="70" t="s">
+        <v>60</v>
+      </c>
+      <c r="B26" s="71" t="s">
+        <v>61</v>
+      </c>
+      <c r="C26" s="71" t="s">
+        <v>62</v>
+      </c>
+      <c r="D26" s="72" t="s">
+        <v>63</v>
+      </c>
+      <c r="E26" s="73" t="s">
+        <v>64</v>
+      </c>
+      <c r="F26" s="73" t="s">
+        <v>65</v>
+      </c>
+      <c r="G26" s="74" t="s">
+        <v>66</v>
+      </c>
+      <c r="H26" s="73" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" ht="41.4">
+      <c r="A27" s="157" t="s">
+        <v>68</v>
+      </c>
+      <c r="B27" s="75">
+        <v>45642</v>
+      </c>
+      <c r="C27" s="76" t="s">
+        <v>69</v>
+      </c>
+      <c r="D27" s="19" t="s">
+        <v>70</v>
+      </c>
+      <c r="E27" s="77" t="s">
+        <v>105</v>
+      </c>
+      <c r="F27" s="78" t="s">
+        <v>41</v>
+      </c>
+      <c r="G27" s="79" t="s">
+        <v>72</v>
+      </c>
+      <c r="H27" s="78" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" ht="41.4">
+      <c r="A28" s="158"/>
+      <c r="B28" s="75">
+        <v>45643</v>
+      </c>
+      <c r="C28" s="76" t="s">
+        <v>93</v>
+      </c>
+      <c r="D28" s="19" t="s">
+        <v>94</v>
+      </c>
+      <c r="E28" s="77" t="s">
+        <v>107</v>
+      </c>
+      <c r="F28" s="78" t="s">
+        <v>41</v>
+      </c>
+      <c r="G28" s="79" t="s">
+        <v>72</v>
+      </c>
+      <c r="H28" s="78" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" ht="55.2">
+      <c r="A29" s="158"/>
+      <c r="B29" s="75">
+        <v>45644</v>
+      </c>
+      <c r="C29" s="76" t="s">
+        <v>97</v>
+      </c>
+      <c r="D29" s="19" t="s">
+        <v>98</v>
+      </c>
+      <c r="E29" s="77" t="s">
+        <v>109</v>
+      </c>
+      <c r="F29" s="78" t="s">
+        <v>41</v>
+      </c>
+      <c r="G29" s="79" t="s">
+        <v>72</v>
+      </c>
+      <c r="H29" s="78" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" ht="55.2">
+      <c r="A30" s="158"/>
+      <c r="B30" s="75">
+        <v>45645</v>
+      </c>
+      <c r="C30" s="76" t="s">
+        <v>101</v>
+      </c>
+      <c r="D30" s="19" t="s">
+        <v>102</v>
+      </c>
+      <c r="E30" s="77" t="s">
+        <v>111</v>
+      </c>
+      <c r="F30" s="78" t="s">
+        <v>41</v>
+      </c>
+      <c r="G30" s="79" t="s">
+        <v>72</v>
+      </c>
+      <c r="H30" s="78" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" ht="28.8">
+      <c r="A31" s="133"/>
+      <c r="B31" s="75">
+        <v>45663</v>
+      </c>
+      <c r="C31" s="76" t="s">
+        <v>69</v>
+      </c>
+      <c r="D31" s="19" t="s">
+        <v>70</v>
+      </c>
+      <c r="E31" s="77" t="s">
+        <v>113</v>
+      </c>
+      <c r="F31" s="78" t="s">
+        <v>75</v>
+      </c>
+      <c r="G31" s="79" t="s">
+        <v>72</v>
+      </c>
+      <c r="H31" s="80" t="s">
+        <v>114</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="5">
+    <mergeCell ref="A27:A31"/>
     <mergeCell ref="A2:H7"/>
     <mergeCell ref="G10:G11"/>
     <mergeCell ref="H10:H11"/>
-    <mergeCell ref="A15:A17"/>
+    <mergeCell ref="A15:A20"/>
   </mergeCells>
   <phoneticPr fontId="40" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>

</xml_diff>